<commit_message>
TP2 , falta UML y revisar casos de prueba
</commit_message>
<xml_diff>
--- a/TP2/PlanillaDeMetricas.xlsx
+++ b/TP2/PlanillaDeMetricas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="20730" windowHeight="10170"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20730" windowHeight="10110"/>
   </bookViews>
   <sheets>
     <sheet name="Métricas" sheetId="2" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>Preparación de la Prueba</t>
   </si>
@@ -110,6 +110,18 @@
   </si>
   <si>
     <t>TP2 - GRUPAL - Sistemas de Ecuaciones Lineales</t>
+  </si>
+  <si>
+    <t>Clase Vector</t>
+  </si>
+  <si>
+    <t>Clase Matriz</t>
+  </si>
+  <si>
+    <t>Clase SEL</t>
+  </si>
+  <si>
+    <t>Paquete Test</t>
   </si>
 </sst>
 </file>
@@ -756,11 +768,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="6" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -771,61 +790,22 @@
     <xf numFmtId="49" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -836,16 +816,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -854,6 +824,48 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="6" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1008,19 +1020,19 @@
                 <c:formatCode>[h]:mm</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>7.6388888888889728E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2.6388888888888906E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1.3888888888888951E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1.0416666666666666E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>8.8888888888888795E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1395,7 +1407,7 @@
   <dimension ref="A1:P58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C1" sqref="C1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1413,29 +1425,29 @@
       <c r="B1" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="80" t="s">
+      <c r="C1" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="63"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="57"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -1461,36 +1473,42 @@
       <c r="E3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="82"/>
-      <c r="N3" s="82"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="65"/>
+      <c r="N3" s="65"/>
       <c r="O3" s="14"/>
       <c r="P3" s="9"/>
     </row>
     <row r="4" spans="1:16" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="33" t="str">
+      <c r="B4" s="45">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="C4" s="46">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="D4" s="46">
+        <v>0.55625000000000002</v>
+      </c>
+      <c r="E4" s="33">
         <f>IFERROR(IF(OR(ISBLANK(C4),ISBLANK(D4)),"Completar",IF(D4&gt;=C4,D4-C4,"Error")),"Error")</f>
-        <v>Completar</v>
-      </c>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="64"/>
-      <c r="M4" s="64"/>
-      <c r="N4" s="64"/>
+        <v>7.6388888888889728E-3</v>
+      </c>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="66"/>
+      <c r="M4" s="66"/>
+      <c r="N4" s="66"/>
       <c r="O4" s="15"/>
       <c r="P4" s="11"/>
     </row>
@@ -1514,12 +1532,12 @@
     </row>
     <row r="6" spans="1:16" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="63"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="57"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -1545,36 +1563,42 @@
       <c r="E7" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="82"/>
-      <c r="L7" s="82"/>
-      <c r="M7" s="82"/>
-      <c r="N7" s="82"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="65"/>
+      <c r="L7" s="65"/>
+      <c r="M7" s="65"/>
+      <c r="N7" s="65"/>
       <c r="O7" s="14"/>
       <c r="P7" s="9"/>
     </row>
     <row r="8" spans="1:16" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="33" t="str">
+      <c r="B8" s="45">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="C8" s="46">
+        <v>0.55694444444444446</v>
+      </c>
+      <c r="D8" s="46">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E8" s="33">
         <f>IFERROR(IF(OR(ISBLANK(C8),ISBLANK(D8)),"Completar",IF(D8&gt;=C8,D8-C8,"Error")),"Error")</f>
-        <v>Completar</v>
-      </c>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="64"/>
-      <c r="K8" s="64"/>
-      <c r="L8" s="64"/>
-      <c r="M8" s="64"/>
-      <c r="N8" s="64"/>
+        <v>2.6388888888888906E-2</v>
+      </c>
+      <c r="F8" s="66"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="66"/>
+      <c r="I8" s="66"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="66"/>
+      <c r="L8" s="66"/>
+      <c r="M8" s="66"/>
+      <c r="N8" s="66"/>
       <c r="O8" s="15"/>
       <c r="P8" s="11"/>
     </row>
@@ -1598,50 +1622,50 @@
     </row>
     <row r="10" spans="1:16" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="62"/>
-      <c r="L10" s="62"/>
-      <c r="M10" s="62"/>
-      <c r="N10" s="63"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="56"/>
+      <c r="M10" s="56"/>
+      <c r="N10" s="57"/>
       <c r="O10" s="13"/>
     </row>
     <row r="11" spans="1:16" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
-      <c r="B11" s="65" t="s">
+      <c r="B11" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="74"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="76" t="s">
+      <c r="D11" s="72"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="77"/>
-      <c r="H11" s="73" t="s">
+      <c r="G11" s="62"/>
+      <c r="H11" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="74"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="76" t="s">
+      <c r="I11" s="72"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="L11" s="77"/>
-      <c r="M11" s="73" t="s">
+      <c r="L11" s="62"/>
+      <c r="M11" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="N11" s="81" t="s">
+      <c r="N11" s="64" t="s">
         <v>2</v>
       </c>
       <c r="O11" s="14"/>
@@ -1649,10 +1673,10 @@
     </row>
     <row r="12" spans="1:16" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
-      <c r="B12" s="65"/>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="75"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="73"/>
       <c r="F12" s="18" t="s">
         <v>13</v>
       </c>
@@ -1674,8 +1698,8 @@
       <c r="L12" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="M12" s="73"/>
-      <c r="N12" s="81"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="64"/>
       <c r="O12" s="14"/>
       <c r="P12" s="9"/>
     </row>
@@ -1685,23 +1709,39 @@
         <f>ROW($B13)-12</f>
         <v>1</v>
       </c>
-      <c r="C13" s="78"/>
-      <c r="D13" s="78"/>
-      <c r="E13" s="79"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="20" t="str">
+      <c r="C13" s="67" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="67"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="47">
+        <v>150</v>
+      </c>
+      <c r="G13" s="48">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="H13" s="49">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="I13" s="50">
+        <v>0.81597222222222221</v>
+      </c>
+      <c r="J13" s="20">
         <f>IFERROR(IF(OR(ISBLANK(H13),ISBLANK(I13)),"Completar",IF(I13&gt;=H13,I13-H13,"Error")),"Error")</f>
-        <v>Completar</v>
-      </c>
-      <c r="K13" s="51"/>
-      <c r="L13" s="52"/>
-      <c r="M13" s="53"/>
-      <c r="N13" s="25" t="str">
+        <v>2.430555555555558E-2</v>
+      </c>
+      <c r="K13" s="51">
+        <v>0</v>
+      </c>
+      <c r="L13" s="52">
+        <v>0</v>
+      </c>
+      <c r="M13" s="53">
+        <v>168</v>
+      </c>
+      <c r="N13" s="25">
         <f>IFERROR(IF(OR(J13="Completar",ISBLANK(L13)),"Completar",J13+L13),"Error")</f>
-        <v>Completar</v>
+        <v>2.430555555555558E-2</v>
       </c>
       <c r="O13" s="15"/>
       <c r="P13" s="11"/>
@@ -1712,50 +1752,82 @@
         <f t="shared" ref="B14:B16" si="0">ROW($B14)-12</f>
         <v>2</v>
       </c>
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="79"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="20" t="str">
+      <c r="C14" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="67"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="47">
+        <v>200</v>
+      </c>
+      <c r="G14" s="48">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="H14" s="49">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="I14" s="50">
+        <v>0.86805555555555547</v>
+      </c>
+      <c r="J14" s="20">
         <f t="shared" ref="J14:J16" si="1">IFERROR(IF(OR(ISBLANK(H14),ISBLANK(I14)),"Completar",IF(I14&gt;=H14,I14-H14,"Error")),"Error")</f>
-        <v>Completar</v>
-      </c>
-      <c r="K14" s="51"/>
-      <c r="L14" s="52"/>
-      <c r="M14" s="53"/>
-      <c r="N14" s="25" t="str">
+        <v>4.513888888888884E-2</v>
+      </c>
+      <c r="K14" s="51">
+        <v>1</v>
+      </c>
+      <c r="L14" s="52">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="M14" s="53">
+        <v>265</v>
+      </c>
+      <c r="N14" s="25">
         <f t="shared" ref="N14:N16" si="2">IFERROR(IF(OR(J14="Completar",ISBLANK(L14)),"Completar",J14+L14),"Error")</f>
-        <v>Completar</v>
+        <v>5.2083333333333287E-2</v>
       </c>
       <c r="O14" s="15"/>
       <c r="P14" s="11"/>
     </row>
-    <row r="15" spans="1:16" s="3" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="24">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C15" s="78"/>
-      <c r="D15" s="78"/>
-      <c r="E15" s="79"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="50"/>
-      <c r="J15" s="20" t="str">
+      <c r="C15" s="67" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="67"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="47">
+        <v>100</v>
+      </c>
+      <c r="G15" s="48">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="H15" s="49">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="I15" s="50">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="J15" s="20">
         <f t="shared" si="1"/>
-        <v>Completar</v>
-      </c>
-      <c r="K15" s="51"/>
-      <c r="L15" s="52"/>
-      <c r="M15" s="53"/>
-      <c r="N15" s="25" t="str">
+        <v>1.388888888888884E-2</v>
+      </c>
+      <c r="K15" s="51">
+        <v>1</v>
+      </c>
+      <c r="L15" s="52">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="M15" s="53">
+        <v>134</v>
+      </c>
+      <c r="N15" s="25">
         <f t="shared" si="2"/>
-        <v>Completar</v>
+        <v>1.7361111111111063E-2</v>
       </c>
       <c r="O15" s="15"/>
       <c r="P15" s="11"/>
@@ -1766,64 +1838,80 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="79"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="20" t="str">
+      <c r="C16" s="67" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="67"/>
+      <c r="E16" s="68"/>
+      <c r="F16" s="47">
+        <v>40</v>
+      </c>
+      <c r="G16" s="48">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="H16" s="49">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="I16" s="50">
+        <v>0.60972222222222217</v>
+      </c>
+      <c r="J16" s="20">
         <f t="shared" si="1"/>
-        <v>Completar</v>
-      </c>
-      <c r="K16" s="51"/>
-      <c r="L16" s="52"/>
-      <c r="M16" s="53"/>
-      <c r="N16" s="25" t="str">
+        <v>5.5555555555555358E-3</v>
+      </c>
+      <c r="K16" s="51">
+        <v>0</v>
+      </c>
+      <c r="L16" s="52">
+        <v>0</v>
+      </c>
+      <c r="M16" s="53">
+        <v>48</v>
+      </c>
+      <c r="N16" s="25">
         <f t="shared" si="2"/>
-        <v>Completar</v>
+        <v>5.5555555555555358E-3</v>
       </c>
       <c r="O16" s="15"/>
       <c r="P16" s="11"/>
     </row>
     <row r="17" spans="1:16" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
-      <c r="B17" s="83" t="s">
+      <c r="B17" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="84"/>
-      <c r="D17" s="84"/>
-      <c r="E17" s="85"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="71"/>
       <c r="F17" s="26">
         <f>SUM(F13:F16)</f>
-        <v>0</v>
+        <v>490</v>
       </c>
       <c r="G17" s="27">
         <f>SUM(G13:G16)</f>
-        <v>0</v>
+        <v>7.9861111111111105E-2</v>
       </c>
       <c r="H17" s="28"/>
       <c r="I17" s="29"/>
-      <c r="J17" s="30" t="str">
+      <c r="J17" s="30">
         <f>IF(OR(COUNTIF(J13:J16,"Error")&gt;0,COUNTIF(J13:J16,"Completar")&gt;0),"Error",SUM(J13:J16))</f>
-        <v>Error</v>
+        <v>8.8888888888888795E-2</v>
       </c>
       <c r="K17" s="31">
         <f>SUM(K13:K16)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L17" s="27">
         <f>SUM(L13:L16)</f>
-        <v>0</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="M17" s="32">
         <f>SUM(M13:M16)</f>
-        <v>0</v>
-      </c>
-      <c r="N17" s="33" t="str">
+        <v>615</v>
+      </c>
+      <c r="N17" s="33">
         <f>IF(OR(COUNTIF(N13:N16,"Error")&gt;0,COUNTIF(N13:N16,"Completar")&gt;0),"Error",SUM(N13:N16))</f>
-        <v>Error</v>
+        <v>9.9305555555555466E-2</v>
       </c>
       <c r="O17" s="14"/>
       <c r="P17" s="17"/>
@@ -1847,12 +1935,12 @@
     </row>
     <row r="19" spans="1:16" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
-      <c r="B19" s="61" t="s">
+      <c r="B19" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="62"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="63"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="57"/>
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
@@ -1892,12 +1980,18 @@
     </row>
     <row r="21" spans="1:16" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15"/>
-      <c r="B21" s="45"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="33" t="str">
+      <c r="B21" s="45">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="C21" s="46">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="D21" s="46">
+        <v>0.625</v>
+      </c>
+      <c r="E21" s="33">
         <f>IFERROR(IF(OR(ISBLANK(C21),ISBLANK(D21)),"Completar",IF(D21&gt;=C21,D21-C21,"Error")),"Error")</f>
-        <v>Completar</v>
+        <v>1.3888888888888951E-2</v>
       </c>
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
@@ -1929,33 +2023,33 @@
       <c r="O22" s="16"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="61" t="s">
+      <c r="B23" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="62"/>
-      <c r="L23" s="62"/>
-      <c r="M23" s="62"/>
-      <c r="N23" s="63"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="56"/>
+      <c r="K23" s="56"/>
+      <c r="L23" s="56"/>
+      <c r="M23" s="56"/>
+      <c r="N23" s="57"/>
     </row>
     <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="56" t="s">
+      <c r="B24" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="57"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="69">
+      <c r="C24" s="59"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="82">
         <f>M17</f>
-        <v>0</v>
-      </c>
-      <c r="F24" s="70"/>
+        <v>615</v>
+      </c>
+      <c r="F24" s="83"/>
       <c r="G24" s="34"/>
       <c r="H24" s="35"/>
       <c r="I24" s="35"/>
@@ -1966,16 +2060,16 @@
       <c r="N24" s="38"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="56" t="s">
+      <c r="B25" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="57"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="71">
+      <c r="C25" s="59"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="84">
         <f>IF(M17=0,0,IFERROR(M17/(N17*24),"Error"))</f>
-        <v>0</v>
-      </c>
-      <c r="F25" s="72"/>
+        <v>258.04195804195831</v>
+      </c>
+      <c r="F25" s="85"/>
       <c r="G25" s="36"/>
       <c r="H25" s="37"/>
       <c r="I25" s="37"/>
@@ -1986,16 +2080,16 @@
       <c r="N25" s="39"/>
     </row>
     <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="56" t="s">
+      <c r="B26" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="57"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="69">
+      <c r="C26" s="59"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="82">
         <f>IF(K17=0,0,IFERROR(ROUNDUP(K17/(M17/100),0),"Error"))</f>
-        <v>0</v>
-      </c>
-      <c r="F26" s="70"/>
+        <v>1</v>
+      </c>
+      <c r="F26" s="83"/>
       <c r="G26" s="36"/>
       <c r="H26" s="37"/>
       <c r="I26" s="37"/>
@@ -2006,16 +2100,16 @@
       <c r="N26" s="39"/>
     </row>
     <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="56" t="s">
+      <c r="B27" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="57"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="54">
+      <c r="C27" s="59"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="74">
         <f>IF(K17=0,0,IFERROR(K17/M17,"Error"))</f>
-        <v>0</v>
-      </c>
-      <c r="F27" s="55"/>
+        <v>3.2520325203252032E-3</v>
+      </c>
+      <c r="F27" s="75"/>
       <c r="G27" s="36"/>
       <c r="H27" s="37"/>
       <c r="I27" s="37"/>
@@ -2026,18 +2120,18 @@
       <c r="N27" s="39"/>
     </row>
     <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="56" t="s">
+      <c r="B28" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="57"/>
-      <c r="D28" s="58"/>
-      <c r="E28" s="43" t="str">
+      <c r="C28" s="59"/>
+      <c r="D28" s="60"/>
+      <c r="E28" s="43">
         <f>E4</f>
-        <v>Completar</v>
-      </c>
-      <c r="F28" s="44" t="str">
+        <v>7.6388888888889728E-3</v>
+      </c>
+      <c r="F28" s="44">
         <f t="shared" ref="F28:F32" si="3">IF(E28="Completar",E28,IFERROR(E28/$E$33,"Error"))</f>
-        <v>Completar</v>
+        <v>5.1886792452830739E-2</v>
       </c>
       <c r="G28" s="36"/>
       <c r="H28" s="37"/>
@@ -2049,18 +2143,18 @@
       <c r="N28" s="39"/>
     </row>
     <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="56" t="s">
+      <c r="B29" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="57"/>
-      <c r="D29" s="58"/>
-      <c r="E29" s="43" t="str">
+      <c r="C29" s="59"/>
+      <c r="D29" s="60"/>
+      <c r="E29" s="43">
         <f>E8</f>
-        <v>Completar</v>
-      </c>
-      <c r="F29" s="44" t="str">
+        <v>2.6388888888888906E-2</v>
+      </c>
+      <c r="F29" s="44">
         <f t="shared" si="3"/>
-        <v>Completar</v>
+        <v>0.17924528301886797</v>
       </c>
       <c r="G29" s="36"/>
       <c r="H29" s="37"/>
@@ -2072,18 +2166,18 @@
       <c r="N29" s="39"/>
     </row>
     <row r="30" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="56" t="s">
+      <c r="B30" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="57"/>
-      <c r="D30" s="58"/>
-      <c r="E30" s="43" t="str">
+      <c r="C30" s="59"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="43">
         <f>E21</f>
-        <v>Completar</v>
-      </c>
-      <c r="F30" s="44" t="str">
+        <v>1.3888888888888951E-2</v>
+      </c>
+      <c r="F30" s="44">
         <f>IF(E30="Completar",E30,IFERROR(E30/$E$33,"Error"))</f>
-        <v>Completar</v>
+        <v>9.4339622641509815E-2</v>
       </c>
       <c r="G30" s="36"/>
       <c r="H30" s="37"/>
@@ -2095,18 +2189,18 @@
       <c r="N30" s="39"/>
     </row>
     <row r="31" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="56" t="s">
+      <c r="B31" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="57"/>
-      <c r="D31" s="58"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="60"/>
       <c r="E31" s="43">
         <f>L17</f>
-        <v>0</v>
-      </c>
-      <c r="F31" s="44" t="str">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="F31" s="44">
         <f t="shared" si="3"/>
-        <v>Error</v>
+        <v>7.0754716981132046E-2</v>
       </c>
       <c r="G31" s="36"/>
       <c r="H31" s="37"/>
@@ -2118,18 +2212,18 @@
       <c r="N31" s="39"/>
     </row>
     <row r="32" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="56" t="s">
+      <c r="B32" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="57"/>
-      <c r="D32" s="58"/>
-      <c r="E32" s="43" t="str">
+      <c r="C32" s="59"/>
+      <c r="D32" s="60"/>
+      <c r="E32" s="43">
         <f>J17</f>
-        <v>Error</v>
-      </c>
-      <c r="F32" s="44" t="str">
+        <v>8.8888888888888795E-2</v>
+      </c>
+      <c r="F32" s="44">
         <f t="shared" si="3"/>
-        <v>Error</v>
+        <v>0.60377358490565947</v>
       </c>
       <c r="G32" s="36"/>
       <c r="H32" s="37"/>
@@ -2141,16 +2235,16 @@
       <c r="N32" s="39"/>
     </row>
     <row r="33" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="66" t="s">
+      <c r="B33" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="67"/>
-      <c r="D33" s="68"/>
-      <c r="E33" s="59" t="str">
+      <c r="C33" s="80"/>
+      <c r="D33" s="81"/>
+      <c r="E33" s="76">
         <f>IF(COUNTIF(E28:E32,"Error")=0,SUM(E28:E32),"Error")</f>
-        <v>Error</v>
-      </c>
-      <c r="F33" s="60"/>
+        <v>0.14722222222222228</v>
+      </c>
+      <c r="F33" s="77"/>
       <c r="G33" s="40"/>
       <c r="H33" s="41"/>
       <c r="I33" s="41"/>
@@ -2191,6 +2285,27 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <mergeCells count="37">
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="B23:N23"/>
+    <mergeCell ref="F4:N4"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="C11:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
     <mergeCell ref="C1:N1"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B2:E2"/>
@@ -2207,27 +2322,6 @@
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="F3:N3"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="C11:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="B23:N23"/>
-    <mergeCell ref="F4:N4"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="H11:J11"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:XFD1048576">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">

</xml_diff>

<commit_message>
TP2, casos de prueba listos
</commit_message>
<xml_diff>
--- a/TP2/PlanillaDeMetricas.xlsx
+++ b/TP2/PlanillaDeMetricas.xlsx
@@ -768,53 +768,95 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="166" fontId="2" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="6" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -824,48 +866,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="6" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1406,8 +1406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:N1"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1425,29 +1425,29 @@
       <c r="B1" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
+      <c r="N1" s="80"/>
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="57"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="63"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -1473,15 +1473,15 @@
       <c r="E3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="82"/>
+      <c r="N3" s="82"/>
       <c r="O3" s="14"/>
       <c r="P3" s="9"/>
     </row>
@@ -1500,15 +1500,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C4),ISBLANK(D4)),"Completar",IF(D4&gt;=C4,D4-C4,"Error")),"Error")</f>
         <v>7.6388888888889728E-3</v>
       </c>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="66"/>
-      <c r="M4" s="66"/>
-      <c r="N4" s="66"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="64"/>
+      <c r="M4" s="64"/>
+      <c r="N4" s="64"/>
       <c r="O4" s="15"/>
       <c r="P4" s="11"/>
     </row>
@@ -1532,12 +1532,12 @@
     </row>
     <row r="6" spans="1:16" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="57"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="63"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -1563,15 +1563,15 @@
       <c r="E7" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="65"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="65"/>
-      <c r="J7" s="65"/>
-      <c r="K7" s="65"/>
-      <c r="L7" s="65"/>
-      <c r="M7" s="65"/>
-      <c r="N7" s="65"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="82"/>
+      <c r="L7" s="82"/>
+      <c r="M7" s="82"/>
+      <c r="N7" s="82"/>
       <c r="O7" s="14"/>
       <c r="P7" s="9"/>
     </row>
@@ -1590,15 +1590,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C8),ISBLANK(D8)),"Completar",IF(D8&gt;=C8,D8-C8,"Error")),"Error")</f>
         <v>2.6388888888888906E-2</v>
       </c>
-      <c r="F8" s="66"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="66"/>
-      <c r="J8" s="66"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="66"/>
-      <c r="M8" s="66"/>
-      <c r="N8" s="66"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="64"/>
+      <c r="L8" s="64"/>
+      <c r="M8" s="64"/>
+      <c r="N8" s="64"/>
       <c r="O8" s="15"/>
       <c r="P8" s="11"/>
     </row>
@@ -1622,50 +1622,50 @@
     </row>
     <row r="10" spans="1:16" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56"/>
-      <c r="L10" s="56"/>
-      <c r="M10" s="56"/>
-      <c r="N10" s="57"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="62"/>
+      <c r="K10" s="62"/>
+      <c r="L10" s="62"/>
+      <c r="M10" s="62"/>
+      <c r="N10" s="63"/>
       <c r="O10" s="13"/>
     </row>
     <row r="11" spans="1:16" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
-      <c r="B11" s="78" t="s">
+      <c r="B11" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="72" t="s">
+      <c r="C11" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="72"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="61" t="s">
+      <c r="D11" s="74"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="62"/>
-      <c r="H11" s="63" t="s">
+      <c r="G11" s="77"/>
+      <c r="H11" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="72"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="61" t="s">
+      <c r="I11" s="74"/>
+      <c r="J11" s="75"/>
+      <c r="K11" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="L11" s="62"/>
-      <c r="M11" s="63" t="s">
+      <c r="L11" s="77"/>
+      <c r="M11" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="N11" s="64" t="s">
+      <c r="N11" s="81" t="s">
         <v>2</v>
       </c>
       <c r="O11" s="14"/>
@@ -1673,10 +1673,10 @@
     </row>
     <row r="12" spans="1:16" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
-      <c r="B12" s="78"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="73"/>
+      <c r="B12" s="65"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="75"/>
       <c r="F12" s="18" t="s">
         <v>13</v>
       </c>
@@ -1698,8 +1698,8 @@
       <c r="L12" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="M12" s="63"/>
-      <c r="N12" s="64"/>
+      <c r="M12" s="73"/>
+      <c r="N12" s="81"/>
       <c r="O12" s="14"/>
       <c r="P12" s="9"/>
     </row>
@@ -1709,11 +1709,11 @@
         <f>ROW($B13)-12</f>
         <v>1</v>
       </c>
-      <c r="C13" s="67" t="s">
+      <c r="C13" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="67"/>
-      <c r="E13" s="68"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="79"/>
       <c r="F13" s="47">
         <v>150</v>
       </c>
@@ -1752,11 +1752,11 @@
         <f t="shared" ref="B14:B16" si="0">ROW($B14)-12</f>
         <v>2</v>
       </c>
-      <c r="C14" s="67" t="s">
+      <c r="C14" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="67"/>
-      <c r="E14" s="68"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="79"/>
       <c r="F14" s="47">
         <v>200</v>
       </c>
@@ -1795,11 +1795,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C15" s="67" t="s">
+      <c r="C15" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="67"/>
-      <c r="E15" s="68"/>
+      <c r="D15" s="78"/>
+      <c r="E15" s="79"/>
       <c r="F15" s="47">
         <v>100</v>
       </c>
@@ -1838,11 +1838,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C16" s="67" t="s">
+      <c r="C16" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="67"/>
-      <c r="E16" s="68"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="79"/>
       <c r="F16" s="47">
         <v>40</v>
       </c>
@@ -1877,12 +1877,12 @@
     </row>
     <row r="17" spans="1:16" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
-      <c r="B17" s="69" t="s">
+      <c r="B17" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="70"/>
-      <c r="D17" s="70"/>
-      <c r="E17" s="71"/>
+      <c r="C17" s="84"/>
+      <c r="D17" s="84"/>
+      <c r="E17" s="85"/>
       <c r="F17" s="26">
         <f>SUM(F13:F16)</f>
         <v>490</v>
@@ -1935,12 +1935,12 @@
     </row>
     <row r="19" spans="1:16" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
-      <c r="B19" s="55" t="s">
+      <c r="B19" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="56"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="57"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="63"/>
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
@@ -2023,33 +2023,33 @@
       <c r="O22" s="16"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="55" t="s">
+      <c r="B23" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="56"/>
-      <c r="H23" s="56"/>
-      <c r="I23" s="56"/>
-      <c r="J23" s="56"/>
-      <c r="K23" s="56"/>
-      <c r="L23" s="56"/>
-      <c r="M23" s="56"/>
-      <c r="N23" s="57"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="62"/>
+      <c r="L23" s="62"/>
+      <c r="M23" s="62"/>
+      <c r="N23" s="63"/>
     </row>
     <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="58" t="s">
+      <c r="B24" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="59"/>
-      <c r="D24" s="60"/>
-      <c r="E24" s="82">
+      <c r="C24" s="57"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="69">
         <f>M17</f>
         <v>615</v>
       </c>
-      <c r="F24" s="83"/>
+      <c r="F24" s="70"/>
       <c r="G24" s="34"/>
       <c r="H24" s="35"/>
       <c r="I24" s="35"/>
@@ -2060,16 +2060,16 @@
       <c r="N24" s="38"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="58" t="s">
+      <c r="B25" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="59"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="84">
+      <c r="C25" s="57"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="71">
         <f>IF(M17=0,0,IFERROR(M17/(N17*24),"Error"))</f>
         <v>258.04195804195831</v>
       </c>
-      <c r="F25" s="85"/>
+      <c r="F25" s="72"/>
       <c r="G25" s="36"/>
       <c r="H25" s="37"/>
       <c r="I25" s="37"/>
@@ -2080,16 +2080,16 @@
       <c r="N25" s="39"/>
     </row>
     <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="58" t="s">
+      <c r="B26" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="59"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="82">
+      <c r="C26" s="57"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="69">
         <f>IF(K17=0,0,IFERROR(ROUNDUP(K17/(M17/100),0),"Error"))</f>
         <v>1</v>
       </c>
-      <c r="F26" s="83"/>
+      <c r="F26" s="70"/>
       <c r="G26" s="36"/>
       <c r="H26" s="37"/>
       <c r="I26" s="37"/>
@@ -2100,16 +2100,16 @@
       <c r="N26" s="39"/>
     </row>
     <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="58" t="s">
+      <c r="B27" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="59"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="74">
+      <c r="C27" s="57"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="54">
         <f>IF(K17=0,0,IFERROR(K17/M17,"Error"))</f>
         <v>3.2520325203252032E-3</v>
       </c>
-      <c r="F27" s="75"/>
+      <c r="F27" s="55"/>
       <c r="G27" s="36"/>
       <c r="H27" s="37"/>
       <c r="I27" s="37"/>
@@ -2120,11 +2120,11 @@
       <c r="N27" s="39"/>
     </row>
     <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="58" t="s">
+      <c r="B28" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="59"/>
-      <c r="D28" s="60"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="58"/>
       <c r="E28" s="43">
         <f>E4</f>
         <v>7.6388888888889728E-3</v>
@@ -2143,11 +2143,11 @@
       <c r="N28" s="39"/>
     </row>
     <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="58" t="s">
+      <c r="B29" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="59"/>
-      <c r="D29" s="60"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="58"/>
       <c r="E29" s="43">
         <f>E8</f>
         <v>2.6388888888888906E-2</v>
@@ -2166,11 +2166,11 @@
       <c r="N29" s="39"/>
     </row>
     <row r="30" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="58" t="s">
+      <c r="B30" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="59"/>
-      <c r="D30" s="60"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="58"/>
       <c r="E30" s="43">
         <f>E21</f>
         <v>1.3888888888888951E-2</v>
@@ -2189,11 +2189,11 @@
       <c r="N30" s="39"/>
     </row>
     <row r="31" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="58" t="s">
+      <c r="B31" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="59"/>
-      <c r="D31" s="60"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="58"/>
       <c r="E31" s="43">
         <f>L17</f>
         <v>1.0416666666666666E-2</v>
@@ -2212,11 +2212,11 @@
       <c r="N31" s="39"/>
     </row>
     <row r="32" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="58" t="s">
+      <c r="B32" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="59"/>
-      <c r="D32" s="60"/>
+      <c r="C32" s="57"/>
+      <c r="D32" s="58"/>
       <c r="E32" s="43">
         <f>J17</f>
         <v>8.8888888888888795E-2</v>
@@ -2235,16 +2235,16 @@
       <c r="N32" s="39"/>
     </row>
     <row r="33" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="79" t="s">
+      <c r="B33" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="80"/>
-      <c r="D33" s="81"/>
-      <c r="E33" s="76">
+      <c r="C33" s="67"/>
+      <c r="D33" s="68"/>
+      <c r="E33" s="59">
         <f>IF(COUNTIF(E28:E32,"Error")=0,SUM(E28:E32),"Error")</f>
         <v>0.14722222222222228</v>
       </c>
-      <c r="F33" s="77"/>
+      <c r="F33" s="60"/>
       <c r="G33" s="40"/>
       <c r="H33" s="41"/>
       <c r="I33" s="41"/>
@@ -2285,6 +2285,27 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <mergeCells count="37">
+    <mergeCell ref="C1:N1"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="F7:N7"/>
+    <mergeCell ref="F8:N8"/>
+    <mergeCell ref="B10:N10"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F3:N3"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="C11:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="E33:F33"/>
@@ -2301,27 +2322,6 @@
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="H11:J11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="C11:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="C1:N1"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="F7:N7"/>
-    <mergeCell ref="F8:N8"/>
-    <mergeCell ref="B10:N10"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F3:N3"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:XFD1048576">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -2332,7 +2332,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="85" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>